<commit_message>
nova verze 4.3.2 - novy instaler, samostatne ip setting
</commit_message>
<xml_diff>
--- a/TRIMAZKON/temp/TRIMAZKON_address_list.xlsx
+++ b/TRIMAZKON/temp/TRIMAZKON_address_list.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,27 +13,19 @@
     <sheet name="projects_bin2" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -53,17 +46,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -426,10 +416,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -437,12 +427,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Domaci Wifi</t>
+          <t>440_Austin</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.1.131</t>
+          <t>10.96.205.240</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -450,24 +440,39 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>FortiClient Austin: 
+pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK
+FH-2050-20
+10.96.205.80</t>
+        </is>
+      </c>
       <c r="E1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>533valeo</t>
+          <t>497_Edcha</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.227.27</t>
+          <t>172.26.7.240</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>FortiClient Edcha Ex2p78kxp30</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -477,7 +482,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>529_Witte</t>
+          <t>503_Witte</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -491,198 +496,6 @@
         </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t>Kamera VS-S160MX :192.168.0.18</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>192.168.1.243</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>518_Valeo</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>192.168.208.242</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>515_ZF Stara kkkBoleslav</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>10.9.250.240</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>NAS - 10.9.250.100Uer:spravce Pass:Jhv*2708 
-User:jhvadmin Pass
-123TPV456</t>
-        </is>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">515_ </t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>192.168.000.000</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>514_Teleflex</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>192.168.14.240</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>PC:192.168.14.240
-CAM: 192.168.14.??NAS:192.168.14.245
-*******************************
-user: Vision
-pass: *Jhv2708</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>511_Teleflex</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>192.168.1.242</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Teleflex d</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>503_Witte</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -698,52 +511,167 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="E3" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>497_Edcha</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>172.26.7.240</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>FortiClient Edcha Ex2p78kxp30</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>511_Teleflex</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.1.242</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Teleflex </t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>514_Teleflex</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.14.240</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PC:192.168.14.240
+CAM: 192.168.14.???
+NAS:192.168.14.245
+*******************************
+user: Vision
+pass: *Jhv2708</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>518_Valeo</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>192.168.208.242</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>529_Witte</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>192.168.0.240</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Kamera VS-S160MX :192.168.0.186</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Domaci Wifi</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>192.168.1.131</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>474 B_Austin</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>10.96.205.175</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>PC:	10.96.205.175
 NAS:	10.96.205.166
@@ -759,37 +687,86 @@
 UVt1@Ex2p78kxp30atD7we@!qGK</t>
         </is>
       </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>515_ZF Stara Boleslav</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10.9.250.240</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100
+User:spravce Pass:Jhv*2708 
+User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
+123TPV456</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>497_Edcha</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>172.26.7.240</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>FortiClient Edcha Ex2p78kxp30</t>
+        </is>
+      </c>
       <c r="E13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>440_Austin</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>10.96.205.240</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>FortiClient Austin: 
-pass:
-1Pm#J@PFIkzM&amp;Q@i 
-UVt1@Ex2p78kxp30atD7we@!qGK
-FH-2050-20
-10.96.205.80</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -815,117 +792,137 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>515_ZF Stara Boleslav</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>10.9.250.240</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NAS - 10.9.250.100
+User:spravce Pass:Jhv*2708 
+User:jhvadmin Pass:jhvadm1n &gt;&gt;&gt; na portu 8080. 
+123TPV456</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>527_Teijin</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10.101.28.176</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>XG-X2900:		10.101.28.175
+OP:		10.101.28.117</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>474 B_Austin</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10.96.205.175</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PC:	10.96.205.175
+NAS:	10.96.205.166
+FH:	10.96.205.154
+	10.96.205.245
+-----------------------------------------
+user:JHV_Vision, omron 
+Pass:*Jhv2708
+---------------------------------------
+FortiClient Austin: 
+Pass:
+1Pm#J@PFIkzM&amp;Q@i 
+UVt1@Ex2p78kxp30atD7we@!qGK</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.1.243</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>514_Teleflex</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>192.168.14.240</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>PC:192.168.14.240
-CAM: 192.168.14.??NAS:192.168.14.245
+CAM: 192.168.14.???
+NAS:192.168.14.245
 *******************************
 user: Vision
 pass: *Jhv2708</t>
-        </is>
-      </c>
-      <c r="E1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>518_Valeo II</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>192.168.1.243</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>527_Teijin</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>10.101.28.176</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>XG-X2900:		10.101.28.175
-OP:		10.101.28.117</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>529_Witte</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>192.168.0.240</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Kamera VS-S160MX :192.168.0.18</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Domaci Wifi</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>192.168.1.131</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -943,10 +940,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -954,17 +951,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>witte</t>
+          <t>514_Teleflex</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>\\192.168.0.192\</t>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Vision</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>*Jhv2708</t>
         </is>
       </c>
     </row>
@@ -988,114 +995,114 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>518_Valeo II</t>
+          <t>515_ZF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>Z</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>\\192.168.1.10\10_vision</t>
+          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>jhv_vision</t>
+          <t>jhvadmin</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Druha sít, ixon</t>
+          <t>jhvadm1n</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>518_Valeo II</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>\\192.168.1.10\10_vision</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Druha sít, ixon</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>518_Valeo</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>jhv_vision</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Jhv*2708</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>první sít, ixon
 \\192.168.208.200\10_vision</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>515_ZF</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>jhvadmin</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>jhvadm1n</t>
-        </is>
-      </c>
-    </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>514_Teleflex</t>
+          <t>474_B Austin</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
+          <t>\\10.96.205.166\DATA</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>jhv_vision</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1103,36 +1110,9 @@
           <t>*Jhv2708</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>474_B Austin</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>\\10.96.205.166\DATA</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>jhv_vision</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>*Jhv2708</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>10.96.205.166
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>10.96.205.166	
 VisionNas_474B	
 						user:JHV_Vision, omron 
 Pass:*Jhv2708</t>
@@ -1161,64 +1141,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>529_Witte</t>
+          <t>Domaci Wifi</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.0.240</t>
+          <t>192.168.1.131</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Kamera VS-S160MX :192.168.0.18</t>
         </is>
       </c>
       <c r="E1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>515_ZF</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Z</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>\\10.9.250.100\08_Project_ZF_515\kamery</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>jhvadmin</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>jhvadm1n</t>
-        </is>
-      </c>
-    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Domaci Wifi</t>
+          <t>511_Teleflex</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.1.131</t>
+          <t>192.168.1.242</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1226,8 +1174,13 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>1</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Teleflex d</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>